<commit_message>
close #162: Add check to report repeated columns of parent indicators in proportionality
</commit_message>
<xml_diff>
--- a/input_data/data_errors_11/proporcionalidades.xlsx
+++ b/input_data/data_errors_11/proporcionalidades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="17">
   <si>
     <t xml:space="preserve">2-2015</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t xml:space="preserve">8-2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9-2015</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -118,6 +115,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,16 +160,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -308,291 +302,288 @@
   </sheetPr>
   <dimension ref="A1:BH6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BC1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BF2" activeCellId="0" sqref="BF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="1" style="1" width="16.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="48" min="13" style="2" width="16.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="60" min="49" style="1" width="16.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="61" style="2" width="16.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="16.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="4" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="4" t="s">
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="4" t="s">
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="4" t="s">
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="4" t="s">
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3" t="s">
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3" t="s">
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="4" t="s">
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
-      <c r="AS1" s="4" t="s">
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AT1" s="3"/>
-      <c r="AU1" s="3"/>
-      <c r="AV1" s="3"/>
-      <c r="AW1" s="3" t="s">
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AX1" s="3"/>
-      <c r="AY1" s="3"/>
-      <c r="AZ1" s="3" t="s">
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="BA1" s="3"/>
-      <c r="BB1" s="3"/>
-      <c r="BC1" s="3" t="s">
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="BD1" s="3"/>
-      <c r="BE1" s="3"/>
-      <c r="BF1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="BG1" s="3"/>
-      <c r="BH1" s="3"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG1" s="2"/>
+      <c r="BH1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AE2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AF2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AG2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AH2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AI2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AK2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AL2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AM2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AN2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AO2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AP2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AR2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AS2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AT2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AU2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AV2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AW2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AX2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AY2" s="3" t="s">
+      <c r="AY2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="AZ2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="BA2" s="3" t="s">
+      <c r="BA2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="BB2" s="3" t="s">
+      <c r="BB2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="BC2" s="3" t="s">
+      <c r="BC2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="BD2" s="3" t="s">
+      <c r="BD2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="BE2" s="3" t="s">
+      <c r="BE2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="BF2" s="3" t="s">
+      <c r="BF2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="BG2" s="3" t="s">
+      <c r="BG2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="BH2" s="3" t="s">
+      <c r="BH2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -613,7 +604,7 @@
         <v>0.442</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0.558</v>
@@ -697,7 +688,7 @@
         <v>0.442</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI3" s="1" t="n">
         <v>0.558</v>
@@ -795,7 +786,7 @@
         <v>0.442</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>0.558</v>
@@ -879,7 +870,7 @@
         <v>0.442</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI4" s="1" t="n">
         <v>0.558</v>
@@ -977,7 +968,7 @@
         <v>0.442</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>0.558</v>
@@ -1061,7 +1052,7 @@
         <v>0.442</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI5" s="1" t="n">
         <v>0.558</v>
@@ -1159,7 +1150,7 @@
         <v>0.442</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>0.558</v>
@@ -1243,7 +1234,7 @@
         <v>0.442</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI6" s="1" t="n">
         <v>0.558</v>

</xml_diff>